<commit_message>
Tutor Profile Student Message
</commit_message>
<xml_diff>
--- a/TestDataXls/Faq.xlsx
+++ b/TestDataXls/Faq.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530F81DC-02A8-447B-A44B-C70F147AB037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F2DEC3-28F5-47BA-B7A0-7AB1E8EAFEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
   <si>
     <t>password</t>
   </si>
@@ -111,7 +111,34 @@
     <t>Mf class 1</t>
   </si>
   <si>
-    <t>PHP session 4</t>
+    <t>Java session 8</t>
+  </si>
+  <si>
+    <t>tutor54@nkt.com</t>
+  </si>
+  <si>
+    <t>paint sess 1</t>
+  </si>
+  <si>
+    <t>paint fix 1</t>
+  </si>
+  <si>
+    <t>paint var 1</t>
+  </si>
+  <si>
+    <t>paint fix 1 ind</t>
+  </si>
+  <si>
+    <t>paint var 1 ind</t>
+  </si>
+  <si>
+    <t>srinivasesaivanan6324@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@1234</t>
+  </si>
+  <si>
+    <t>clarinet session 4 multi</t>
   </si>
 </sst>
 </file>
@@ -509,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,7 +699,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -687,6 +714,167 @@
         <v>31</v>
       </c>
       <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14">
         <v>5</v>
       </c>
     </row>
@@ -702,9 +890,22 @@
     <hyperlink ref="D6" r:id="rId8" xr:uid="{848A2643-F1B5-4BB6-93AE-7E20788F414F}"/>
     <hyperlink ref="D7" r:id="rId9" xr:uid="{42130E15-03CC-4FBA-9C04-2A8D8C9F6660}"/>
     <hyperlink ref="E7" r:id="rId10" xr:uid="{7450F6D4-7730-4727-BCAB-E60A87CA83F3}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{4A5580EC-259C-4942-939F-9E100227080E}"/>
+    <hyperlink ref="E8" r:id="rId12" xr:uid="{2C5A19E4-0B34-4220-8957-46D020E902D3}"/>
+    <hyperlink ref="D9" r:id="rId13" xr:uid="{E97EA586-1968-470E-9C4C-A37EB0AFA148}"/>
+    <hyperlink ref="E9" r:id="rId14" xr:uid="{41A88FF1-8412-4FB5-87B5-3D7B8345B895}"/>
+    <hyperlink ref="D10" r:id="rId15" xr:uid="{81CF06AE-AE5F-4F23-A9BC-EC84941C84FE}"/>
+    <hyperlink ref="E10" r:id="rId16" xr:uid="{D9F6F41F-7677-47DD-9A1F-64F9B11A6971}"/>
+    <hyperlink ref="E11" r:id="rId17" xr:uid="{B8F8D3A3-DBC9-407D-8BB9-1EBDB28952C9}"/>
+    <hyperlink ref="D12" r:id="rId18" xr:uid="{CF6FFB0C-1E9E-44B3-AC10-536548D4DDE0}"/>
+    <hyperlink ref="E12" r:id="rId19" xr:uid="{2DFBA57D-38E7-485E-9B36-1B2502B8A023}"/>
+    <hyperlink ref="D13" r:id="rId20" xr:uid="{4F5639AF-2D20-4AA2-9A15-23C28FB182E8}"/>
+    <hyperlink ref="E13" r:id="rId21" xr:uid="{C5F453DE-1480-430E-980C-64802502D9F2}"/>
+    <hyperlink ref="D14" r:id="rId22" xr:uid="{763DCF47-E9BC-4AFE-99D7-900EF8473F9D}"/>
+    <hyperlink ref="E14" r:id="rId23" xr:uid="{727D1F57-86BA-4BFF-9CF8-F3D921AB740F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>